<commit_message>
Add R script to generate sample Gantt chart data in Excel
</commit_message>
<xml_diff>
--- a/gantt.xlsx
+++ b/gantt.xlsx
@@ -1,52 +1,69 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0057769\Desktop\dev\powerbiProject\gantt_chart_project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0B82DE4-B57E-4668-AC97-E58DC394DF27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23205" yWindow="3030" windowWidth="14400" windowHeight="8175" xr2:uid="{096BBFCB-1509-4A0C-8F17-53B05F54B468}"/>
+    <workbookView xWindow="-23205" yWindow="3030" windowWidth="14400" windowHeight="8175" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>sample gantt</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start_Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End_Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirement Analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pending</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deployment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,11 +73,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="6"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="游ゴシック"/>
-      <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,17 +96,14 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -422,22 +434,126 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04FE31B-73C9-44D3-9DE0-4BED8ECBE7F9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="25.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="15.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="15.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="15.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="10.71" hidden="0" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>45200</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>45208</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>45209</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>45223</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>45224</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>45244</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>45245</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>45254</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>45255</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>45260</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>